<commit_message>
uploading the block functionality
</commit_message>
<xml_diff>
--- a/Scriptoria project information/scriptoria backlog.xlsx
+++ b/Scriptoria project information/scriptoria backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS-20230610T091643Z-001\VS\university\WEB2\Scriptoria\Scriptoria project information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D65207-D28C-4332-85B6-73C8805A121E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDBEF68-736A-47E1-8972-3B03A1B057A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="85">
   <si>
     <t>As a...</t>
   </si>
@@ -274,6 +274,21 @@
   </si>
   <si>
     <t xml:space="preserve">My account is secured </t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read stories </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can read stories without signing up </t>
+  </si>
+  <si>
+    <t>browse in multi-languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can understand everything </t>
   </si>
 </sst>
 </file>
@@ -728,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1464,6 +1479,43 @@
         <v>28</v>
       </c>
     </row>
+    <row r="34" spans="1:7">
+      <c r="B34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="B35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing the search apge
</commit_message>
<xml_diff>
--- a/Scriptoria project information/scriptoria backlog.xlsx
+++ b/Scriptoria project information/scriptoria backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS-20230610T091643Z-001\VS\university\WEB2\Scriptoria\Scriptoria project information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDBEF68-736A-47E1-8972-3B03A1B057A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038924DE-5A2E-4A9F-A6A4-67482DBC4255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="91">
   <si>
     <t>As a...</t>
   </si>
@@ -147,12 +147,6 @@
     <t>I can easily see if i have any new messages.</t>
   </si>
   <si>
-    <t>Translate button</t>
-  </si>
-  <si>
-    <t>I can change the website language.</t>
-  </si>
-  <si>
     <t xml:space="preserve">User </t>
   </si>
   <si>
@@ -213,12 +207,6 @@
     <t>I don’t share anymore of my personal information</t>
   </si>
   <si>
-    <t xml:space="preserve">I can come back anytime and find it easily </t>
-  </si>
-  <si>
-    <t>Create stories list</t>
-  </si>
-  <si>
     <t>Share my stories list</t>
   </si>
   <si>
@@ -237,15 +225,6 @@
     <t xml:space="preserve">As a user I want to be able to edit my story after I publish it </t>
   </si>
   <si>
-    <t xml:space="preserve">Writer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">track my stories spread in the community </t>
-  </si>
-  <si>
-    <t>I can get some feedback on stories and the way I write</t>
-  </si>
-  <si>
     <t xml:space="preserve">In progress </t>
   </si>
   <si>
@@ -289,6 +268,45 @@
   </si>
   <si>
     <t xml:space="preserve">I can understand everything </t>
+  </si>
+  <si>
+    <t>I can remember it later</t>
+  </si>
+  <si>
+    <t>I can come back anytime and edit it</t>
+  </si>
+  <si>
+    <t>مرشح للسبرنت الرابع</t>
+  </si>
+  <si>
+    <t>have a list of my works</t>
+  </si>
+  <si>
+    <t>Have a reading list</t>
+  </si>
+  <si>
+    <t>Maintenance page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I know if im doing something wrong or the servers are down </t>
+  </si>
+  <si>
+    <t>Search not found page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">so that I know that there is no result for my search </t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -743,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="E41" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -758,11 +776,12 @@
     <col min="5" max="5" width="24.375" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="16.75" customWidth="1"/>
+    <col min="8" max="8" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -797,7 +816,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -820,7 +839,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -843,7 +862,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -866,7 +885,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -889,7 +908,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -912,7 +931,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -929,13 +948,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -958,7 +977,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F9" s="1">
         <v>2</v>
@@ -981,7 +1000,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
@@ -1004,7 +1023,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
@@ -1021,13 +1040,13 @@
         <v>23</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" s="7">
         <v>2</v>
@@ -1040,23 +1059,23 @@
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>70</v>
+      <c r="B13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1067,19 +1086,19 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F14" s="1">
         <v>3</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1090,19 +1109,17 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="1">
-        <v>3</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>70</v>
+        <v>42</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1113,107 +1130,114 @@
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" s="1">
         <v>3</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>41</v>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="7">
+        <v>42</v>
+      </c>
+      <c r="F17" s="1">
         <v>3</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="G17" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s">
-        <v>36</v>
+      <c r="B18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>43</v>
+      </c>
+      <c r="F18" s="7">
+        <v>3</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
+      <c r="B19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>42</v>
+      </c>
+      <c r="F19" s="9">
+        <v>3</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
+      <c r="B20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>42</v>
+      </c>
+      <c r="F20" s="9">
+        <v>3</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1221,39 +1245,44 @@
         <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>45</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F22" s="1"/>
       <c r="G22" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1261,19 +1290,19 @@
         <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>43</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1281,19 +1310,19 @@
         <v>6</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1301,19 +1330,19 @@
         <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>42</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1321,19 +1350,22 @@
         <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1341,19 +1373,19 @@
         <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1361,39 +1393,39 @@
         <v>6</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1401,22 +1433,19 @@
         <v>6</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="2">
-        <v>3</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="G30" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1424,22 +1453,22 @@
         <v>6</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="2">
-        <v>3</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>42</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1453,13 +1482,16 @@
         <v>77</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1467,39 +1499,49 @@
         <v>6</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" t="s">
         <v>78</v>
       </c>
-      <c r="D33" t="s">
-        <v>79</v>
-      </c>
       <c r="E33" s="7" t="s">
-        <v>44</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F33" s="9"/>
       <c r="G33" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
       <c r="B34" s="2" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="1">
-        <v>2</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>42</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
       <c r="B35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1510,10 +1552,33 @@
         <v>84</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>28</v>
+      </c>
+      <c r="H35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="B36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding Arabic transelation to the website
</commit_message>
<xml_diff>
--- a/Scriptoria project information/scriptoria backlog.xlsx
+++ b/Scriptoria project information/scriptoria backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS-20230610T091643Z-001\VS\university\WEB2\Scriptoria\Scriptoria project information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038924DE-5A2E-4A9F-A6A4-67482DBC4255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1336444-3CD1-4E46-8798-FAC07AA4BDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="99">
   <si>
     <t>As a...</t>
   </si>
@@ -141,12 +141,6 @@
     <t>I can get the stories that I'm interested in and I want to read.</t>
   </si>
   <si>
-    <t>Inbox messages button</t>
-  </si>
-  <si>
-    <t>I can easily see if i have any new messages.</t>
-  </si>
-  <si>
     <t xml:space="preserve">User </t>
   </si>
   <si>
@@ -213,9 +207,6 @@
     <t>Everyone that has the same mindset can see it or read it with me</t>
   </si>
   <si>
-    <t>Go the help page</t>
-  </si>
-  <si>
     <t xml:space="preserve">If I have any problem I can contact the help center and they will help me </t>
   </si>
   <si>
@@ -276,9 +267,6 @@
     <t>I can come back anytime and edit it</t>
   </si>
   <si>
-    <t>مرشح للسبرنت الرابع</t>
-  </si>
-  <si>
     <t>have a list of my works</t>
   </si>
   <si>
@@ -297,16 +285,52 @@
     <t xml:space="preserve">so that I know that there is no result for my search </t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
+    <t xml:space="preserve">Dark theme </t>
+  </si>
+  <si>
+    <t>help center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can feel more comfy </t>
+  </si>
+  <si>
+    <t>04/03/2024 - 10/03/2024</t>
+  </si>
+  <si>
+    <t>10/03/2024 - 24/03/2024</t>
+  </si>
+  <si>
+    <t>27/03/2024 - 04/04/2024</t>
+  </si>
+  <si>
+    <t>04/04/2024 - 20/04/2024</t>
+  </si>
+  <si>
+    <t>Date DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>امجد</t>
+  </si>
+  <si>
+    <t>عمر</t>
+  </si>
+  <si>
+    <t>محمد علي</t>
+  </si>
+  <si>
+    <t>عرين</t>
+  </si>
+  <si>
+    <t>لمى</t>
+  </si>
+  <si>
+    <t>عبود</t>
+  </si>
+  <si>
+    <t>احمد</t>
   </si>
 </sst>
 </file>
@@ -335,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,12 +388,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF8ED973"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -421,11 +439,11 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -761,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E41" sqref="A1:XFD1048576"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -776,12 +794,12 @@
     <col min="5" max="5" width="24.375" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="16.75" customWidth="1"/>
-    <col min="8" max="8" width="18.25" customWidth="1"/>
+    <col min="8" max="8" width="23.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -801,8 +819,11 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -816,7 +837,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -824,8 +845,11 @@
       <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -839,7 +863,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -847,8 +871,11 @@
       <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -862,7 +889,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -870,8 +897,11 @@
       <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -885,7 +915,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -893,8 +923,11 @@
       <c r="G5" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -908,7 +941,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -916,8 +949,11 @@
       <c r="G6" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -931,7 +967,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -939,8 +975,11 @@
       <c r="G7" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -948,13 +987,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -962,8 +1001,11 @@
       <c r="G8" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -977,7 +1019,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F9" s="1">
         <v>2</v>
@@ -985,8 +1027,11 @@
       <c r="G9" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1000,7 +1045,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
@@ -1008,8 +1053,11 @@
       <c r="G10" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1023,7 +1071,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
@@ -1031,8 +1079,11 @@
       <c r="G11" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1040,13 +1091,13 @@
         <v>23</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F12" s="7">
         <v>2</v>
@@ -1054,22 +1105,25 @@
       <c r="G12" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F13" s="7">
         <v>2</v>
@@ -1077,8 +1131,11 @@
       <c r="G13" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1092,37 +1149,45 @@
         <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F14" s="1">
         <v>3</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="G14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
+      <c r="B15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>41</v>
+      </c>
+      <c r="F15" s="7">
+        <v>3</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1130,22 +1195,25 @@
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="1">
+        <v>40</v>
+      </c>
+      <c r="F16" s="9">
         <v>3</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>60</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1153,45 +1221,51 @@
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="9">
         <v>3</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="G17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>39</v>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="7">
+        <v>41</v>
+      </c>
+      <c r="F18" s="9">
         <v>3</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="G18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1199,22 +1273,25 @@
         <v>6</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F19" s="9">
         <v>3</v>
       </c>
-      <c r="G19" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="G19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1222,22 +1299,25 @@
         <v>6</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F20" s="9">
         <v>3</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="G20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1245,64 +1325,80 @@
         <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>40</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>42</v>
+      </c>
+      <c r="F23" s="1">
+        <v>4</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1310,19 +1406,28 @@
         <v>6</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>42</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1330,19 +1435,28 @@
         <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>40</v>
+      </c>
+      <c r="F25" s="1">
+        <v>4</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1350,22 +1464,28 @@
         <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>40</v>
+      </c>
+      <c r="F26" s="1">
+        <v>4</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1373,19 +1493,28 @@
         <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>40</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1393,19 +1522,28 @@
         <v>6</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="1">
+        <v>4</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="H28" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1413,19 +1551,28 @@
         <v>6</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>40</v>
+      </c>
+      <c r="F29" s="1">
+        <v>4</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1433,19 +1580,28 @@
         <v>6</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>40</v>
+      </c>
+      <c r="F30" s="1">
+        <v>4</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1453,10 +1609,10 @@
         <v>6</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>42</v>
@@ -1464,11 +1620,8 @@
       <c r="G31" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1476,22 +1629,19 @@
         <v>6</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1499,23 +1649,19 @@
         <v>6</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F33" s="9"/>
       <c r="G33" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1523,22 +1669,19 @@
         <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D34" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1546,10 +1689,10 @@
         <v>6</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>42</v>
@@ -1557,28 +1700,32 @@
       <c r="G35" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
       <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>42</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F36" s="1"/>
       <c r="G36" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H36" t="s">
-        <v>80</v>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding fixing something in the homepage
</commit_message>
<xml_diff>
--- a/Scriptoria project information/scriptoria backlog.xlsx
+++ b/Scriptoria project information/scriptoria backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS-20230610T091643Z-001\VS\university\WEB2\Scriptoria\Scriptoria project information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1336444-3CD1-4E46-8798-FAC07AA4BDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFF9618-DD63-442C-98C6-AEA8E419C3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="102">
   <si>
     <t>As a...</t>
   </si>
@@ -327,10 +327,19 @@
     <t>لمى</t>
   </si>
   <si>
+    <t>احمد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عبود </t>
+  </si>
+  <si>
+    <t>20/04/2024-20/5/2024</t>
+  </si>
+  <si>
+    <t>امجد وعمر</t>
+  </si>
+  <si>
     <t>عبود</t>
-  </si>
-  <si>
-    <t>احمد</t>
   </si>
 </sst>
 </file>
@@ -781,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1180,8 +1189,8 @@
       <c r="F15" s="7">
         <v>3</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>60</v>
+      <c r="G15" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>89</v>
@@ -1206,8 +1215,8 @@
       <c r="F16" s="9">
         <v>3</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>60</v>
+      <c r="G16" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>89</v>
@@ -1620,6 +1629,9 @@
       <c r="G31" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="I31" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2">
@@ -1640,8 +1652,11 @@
       <c r="G32" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="I32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1660,8 +1675,11 @@
       <c r="G33" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="I33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1680,8 +1698,11 @@
       <c r="G34" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="I34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1700,8 +1721,11 @@
       <c r="G35" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="I35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1717,12 +1741,20 @@
       <c r="E36" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="F36" s="1">
+        <v>5</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="2"/>
       <c r="C37" s="2" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
alllah yl3n githup servers
</commit_message>
<xml_diff>
--- a/Scriptoria project information/scriptoria backlog.xlsx
+++ b/Scriptoria project information/scriptoria backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS-20230610T091643Z-001\VS\university\WEB2\Scriptoria\Scriptoria project information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C835978A-4369-47EE-81CE-0DB33C87B7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C374D30-79EE-4EEE-B67F-81629F41A2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1626,6 +1626,9 @@
       <c r="E31" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="F31" s="1">
+        <v>5</v>
+      </c>
       <c r="G31" s="8" t="s">
         <v>28</v>
       </c>
@@ -1649,6 +1652,9 @@
       <c r="E32" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="F32" s="1">
+        <v>5</v>
+      </c>
       <c r="G32" s="8" t="s">
         <v>28</v>
       </c>
@@ -1672,6 +1678,9 @@
       <c r="E33" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="F33" s="1">
+        <v>5</v>
+      </c>
       <c r="G33" s="8" t="s">
         <v>28</v>
       </c>
@@ -1695,6 +1704,9 @@
       <c r="E34" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="F34" s="1">
+        <v>5</v>
+      </c>
       <c r="G34" s="8" t="s">
         <v>28</v>
       </c>
@@ -1717,6 +1729,9 @@
       </c>
       <c r="E35" s="7" t="s">
         <v>42</v>
+      </c>
+      <c r="F35" s="1">
+        <v>5</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
removing the follow when the user blocks another user
</commit_message>
<xml_diff>
--- a/Scriptoria project information/scriptoria backlog.xlsx
+++ b/Scriptoria project information/scriptoria backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS-20230610T091643Z-001\VS\university\WEB2\Scriptoria\Scriptoria project information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399FDB9C-481D-4B72-9B48-DE0CAA2ACD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3111B99F-E677-499C-9874-9465BD844194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="94">
   <si>
     <t>As a...</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t xml:space="preserve">As a user I want to be able to edit my story after I publish it </t>
-  </si>
-  <si>
-    <t xml:space="preserve">In progress </t>
   </si>
   <si>
     <t>ID</t>
@@ -347,7 +344,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,12 +369,6 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF1A983"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -391,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -416,9 +407,6 @@
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -760,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -778,7 +766,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -799,7 +787,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -824,8 +812,8 @@
       <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>83</v>
+      <c r="H2" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -850,8 +838,8 @@
       <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>83</v>
+      <c r="H3" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -876,8 +864,8 @@
       <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>83</v>
+      <c r="H4" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -902,8 +890,8 @@
       <c r="G5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>83</v>
+      <c r="H5" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -928,8 +916,8 @@
       <c r="G6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>83</v>
+      <c r="H6" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -954,8 +942,8 @@
       <c r="G7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>83</v>
+      <c r="H7" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -980,8 +968,8 @@
       <c r="G8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>83</v>
+      <c r="H8" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1007,7 +995,7 @@
         <v>9</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1033,7 +1021,7 @@
         <v>9</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1059,7 +1047,7 @@
         <v>9</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1085,7 +1073,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1093,13 +1081,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>39</v>
@@ -1111,7 +1099,7 @@
         <v>9</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1137,7 +1125,7 @@
         <v>9</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1163,7 +1151,7 @@
         <v>9</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1189,7 +1177,7 @@
         <v>9</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1200,7 +1188,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
         <v>56</v>
@@ -1215,7 +1203,7 @@
         <v>9</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1241,7 +1229,7 @@
         <v>9</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1252,10 +1240,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>39</v>
@@ -1267,7 +1255,7 @@
         <v>9</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1278,10 +1266,10 @@
         <v>6</v>
       </c>
       <c r="C20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>39</v>
@@ -1293,7 +1281,7 @@
         <v>9</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1319,7 +1307,7 @@
         <v>9</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1345,7 +1333,7 @@
         <v>9</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1371,7 +1359,7 @@
         <v>9</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1397,7 +1385,7 @@
         <v>9</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1408,10 +1396,10 @@
         <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
         <v>65</v>
-      </c>
-      <c r="D25" t="s">
-        <v>66</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>39</v>
@@ -1423,7 +1411,7 @@
         <v>9</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1434,10 +1422,10 @@
         <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
         <v>70</v>
-      </c>
-      <c r="D26" t="s">
-        <v>71</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>39</v>
@@ -1449,7 +1437,7 @@
         <v>9</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1460,10 +1448,10 @@
         <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>39</v>
@@ -1475,7 +1463,7 @@
         <v>9</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1486,10 +1474,10 @@
         <v>6</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>39</v>
@@ -1501,7 +1489,7 @@
         <v>9</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1512,10 +1500,10 @@
         <v>6</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" t="s">
         <v>76</v>
-      </c>
-      <c r="D29" t="s">
-        <v>77</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>39</v>
@@ -1527,7 +1515,7 @@
         <v>9</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1538,10 +1526,10 @@
         <v>6</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" t="s">
         <v>78</v>
-      </c>
-      <c r="D30" t="s">
-        <v>79</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>39</v>
@@ -1553,7 +1541,7 @@
         <v>9</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1575,11 +1563,11 @@
       <c r="F31" s="7">
         <v>5</v>
       </c>
-      <c r="G31" s="10" t="s">
-        <v>59</v>
+      <c r="G31" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1605,7 +1593,7 @@
         <v>9</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1631,7 +1619,7 @@
         <v>9</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1642,10 +1630,10 @@
         <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>41</v>
@@ -1653,11 +1641,11 @@
       <c r="F34" s="1">
         <v>5</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>59</v>
+      <c r="G34" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1679,11 +1667,11 @@
       <c r="F35" s="1">
         <v>5</v>
       </c>
-      <c r="G35" s="10" t="s">
-        <v>59</v>
+      <c r="G35" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1694,43 +1682,43 @@
         <v>6</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" t="s">
         <v>89</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="F36" s="1">
         <v>5</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>59</v>
+      <c r="G36" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="2"/>
       <c r="C37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" t="s">
         <v>92</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="F37" s="1">
         <v>5</v>
       </c>
-      <c r="G37" s="10" t="s">
-        <v>59</v>
+      <c r="G37" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>